<commit_message>
640	Move check answer
</commit_message>
<xml_diff>
--- a/npbenchmark-main/SDK.VRPTW2d/variables.xlsx
+++ b/npbenchmark-main/SDK.VRPTW2d/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\SDK.VRPTW2d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F106D1B-D33B-45C8-A29A-3C85AE0F9EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA4B15B-CDFA-4421-971E-782B1372C1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>java</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2576,6 +2576,29 @@
         <family val="2"/>
       </rPr>
       <t>ACS_Strategy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00627A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>print_result</t>
     </r>
     <r>
       <rPr>
@@ -3184,7 +3207,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3260,9 +3283,15 @@
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>